<commit_message>
Refactor PDF generation and chart handling
Removed Plotly dependency from pdf_generator.py and now expects chart image to be generated externally. Updated PDF report to insert chart image if available, improved table and footer styling, and centralized title. In transformer.py, chart data preparation now aggregates both 'faturamento' and 'custos'. In visualizer.py, switched to logger for messages and removed problematic emoji. Updated logs and regenerated output files to reflect these changes.
</commit_message>
<xml_diff>
--- a/data/reports/relatorio_financeiro.xlsx
+++ b/data/reports/relatorio_financeiro.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -46,8 +48,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -439,10 +442,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2025-01-01</t>
-        </is>
+      <c r="A2" s="1" t="n">
+        <v>45658</v>
       </c>
       <c r="B2" t="n">
         <v>2500</v>
@@ -452,10 +453,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-01-02</t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>45659</v>
       </c>
       <c r="B3" t="n">
         <v>3000</v>
@@ -465,10 +464,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2025-01-03</t>
-        </is>
+      <c r="A4" s="1" t="n">
+        <v>45660</v>
       </c>
       <c r="B4" t="n">
         <v>2000</v>

</xml_diff>